<commit_message>
- minor update to docs - updates to some dashboard for scenario selection
</commit_message>
<xml_diff>
--- a/docs/data_prep/population/proj_19rp3_page_spreadsheet.xlsx
+++ b/docs/data_prep/population/proj_19rp3_page_spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RenderNew\docs\data_prep\population\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2516DF4C-848A-493C-9265-43808BC2889C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC47CF9-2C20-42B1-82A4-B65C64EFAFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -1652,11 +1652,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2072,22 +2072,22 @@
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -17346,10 +17346,10 @@
   <dimension ref="A1:T416"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="12" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="12" topLeftCell="B365" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="W26" sqref="W26"/>
+      <selection pane="bottomRight" activeCell="I415" sqref="I415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17546,35 +17546,35 @@
       <c r="L13" t="s">
         <v>451</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13" s="17">
         <f>SUMIF($J$13:$J$413,$L13,B$13:B$413)</f>
         <v>4237503</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13" s="17">
         <f t="shared" ref="N13:T28" si="1">SUMIF($J$13:$J$413,$L13,C$13:C$413)</f>
         <v>4241757</v>
       </c>
-      <c r="O13" s="19">
+      <c r="O13" s="17">
         <f t="shared" si="1"/>
         <v>4237136</v>
       </c>
-      <c r="P13" s="19">
+      <c r="P13" s="17">
         <f t="shared" si="1"/>
         <v>4227365</v>
       </c>
-      <c r="Q13" s="19">
+      <c r="Q13" s="17">
         <f t="shared" si="1"/>
         <v>4215890</v>
       </c>
-      <c r="R13" s="19">
+      <c r="R13" s="17">
         <f t="shared" si="1"/>
         <v>4196565</v>
       </c>
-      <c r="S13" s="19">
+      <c r="S13" s="17">
         <f t="shared" si="1"/>
         <v>4154041</v>
       </c>
-      <c r="T13" s="19">
+      <c r="T13" s="17">
         <f t="shared" si="1"/>
         <v>4143418</v>
       </c>
@@ -17614,35 +17614,35 @@
       <c r="L14" t="s">
         <v>452</v>
       </c>
-      <c r="M14" s="19">
+      <c r="M14" s="17">
         <f t="shared" ref="M14:M50" si="3">SUMIF($J$13:$J$413,$L14,B$13:B$413)</f>
         <v>2931812</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="17">
         <f t="shared" si="1"/>
         <v>2935574</v>
       </c>
-      <c r="O14" s="19">
+      <c r="O14" s="17">
         <f t="shared" si="1"/>
         <v>2930838</v>
       </c>
-      <c r="P14" s="19">
+      <c r="P14" s="17">
         <f t="shared" si="1"/>
         <v>2918715</v>
       </c>
-      <c r="Q14" s="19">
+      <c r="Q14" s="17">
         <f t="shared" si="1"/>
         <v>2900094</v>
       </c>
-      <c r="R14" s="19">
+      <c r="R14" s="17">
         <f t="shared" si="1"/>
         <v>2871371</v>
       </c>
-      <c r="S14" s="19">
+      <c r="S14" s="17">
         <f t="shared" si="1"/>
         <v>2818551</v>
       </c>
-      <c r="T14" s="19">
+      <c r="T14" s="17">
         <f t="shared" si="1"/>
         <v>2805129</v>
       </c>
@@ -17682,35 +17682,35 @@
       <c r="L15" t="s">
         <v>453</v>
       </c>
-      <c r="M15" s="19">
+      <c r="M15" s="17">
         <f t="shared" si="3"/>
         <v>2262471</v>
       </c>
-      <c r="N15" s="19">
+      <c r="N15" s="17">
         <f t="shared" si="1"/>
         <v>2269648</v>
       </c>
-      <c r="O15" s="19">
+      <c r="O15" s="17">
         <f t="shared" si="1"/>
         <v>2272840</v>
       </c>
-      <c r="P15" s="19">
+      <c r="P15" s="17">
         <f t="shared" si="1"/>
         <v>2273997</v>
       </c>
-      <c r="Q15" s="19">
+      <c r="Q15" s="17">
         <f t="shared" si="1"/>
         <v>2275241</v>
       </c>
-      <c r="R15" s="19">
+      <c r="R15" s="17">
         <f t="shared" si="1"/>
         <v>2275723</v>
       </c>
-      <c r="S15" s="19">
+      <c r="S15" s="17">
         <f t="shared" si="1"/>
         <v>2266942</v>
       </c>
-      <c r="T15" s="19">
+      <c r="T15" s="17">
         <f t="shared" si="1"/>
         <v>2264469</v>
       </c>
@@ -17750,35 +17750,35 @@
       <c r="L16" t="s">
         <v>454</v>
       </c>
-      <c r="M16" s="19">
+      <c r="M16" s="17">
         <f t="shared" si="3"/>
         <v>1924416</v>
       </c>
-      <c r="N16" s="19">
+      <c r="N16" s="17">
         <f t="shared" si="1"/>
         <v>1926453</v>
       </c>
-      <c r="O16" s="19">
+      <c r="O16" s="17">
         <f t="shared" si="1"/>
         <v>1923302</v>
       </c>
-      <c r="P16" s="19">
+      <c r="P16" s="17">
         <f t="shared" si="1"/>
         <v>1915860</v>
       </c>
-      <c r="Q16" s="19">
+      <c r="Q16" s="17">
         <f t="shared" si="1"/>
         <v>1905156</v>
       </c>
-      <c r="R16" s="19">
+      <c r="R16" s="17">
         <f t="shared" si="1"/>
         <v>1889725</v>
       </c>
-      <c r="S16" s="19">
+      <c r="S16" s="17">
         <f t="shared" si="1"/>
         <v>1863259</v>
       </c>
-      <c r="T16" s="19">
+      <c r="T16" s="17">
         <f t="shared" si="1"/>
         <v>1856517</v>
       </c>
@@ -17818,35 +17818,35 @@
       <c r="L17" t="s">
         <v>455</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="17">
         <f t="shared" si="3"/>
         <v>4920457</v>
       </c>
-      <c r="N17" s="19">
+      <c r="N17" s="17">
         <f t="shared" si="1"/>
         <v>4909866</v>
       </c>
-      <c r="O17" s="19">
+      <c r="O17" s="17">
         <f t="shared" si="1"/>
         <v>4892319</v>
       </c>
-      <c r="P17" s="19">
+      <c r="P17" s="17">
         <f t="shared" si="1"/>
         <v>4871324</v>
       </c>
-      <c r="Q17" s="19">
+      <c r="Q17" s="17">
         <f t="shared" si="1"/>
         <v>4842560</v>
       </c>
-      <c r="R17" s="19">
+      <c r="R17" s="17">
         <f t="shared" si="1"/>
         <v>4794020</v>
       </c>
-      <c r="S17" s="19">
+      <c r="S17" s="17">
         <f t="shared" si="1"/>
         <v>4706421</v>
       </c>
-      <c r="T17" s="19">
+      <c r="T17" s="17">
         <f t="shared" si="1"/>
         <v>4686163</v>
       </c>
@@ -17886,35 +17886,35 @@
       <c r="L18" t="s">
         <v>456</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="17">
         <f t="shared" si="3"/>
         <v>1240756</v>
       </c>
-      <c r="N18" s="19">
+      <c r="N18" s="17">
         <f t="shared" si="1"/>
         <v>1246588</v>
       </c>
-      <c r="O18" s="19">
+      <c r="O18" s="17">
         <f t="shared" si="1"/>
         <v>1249789</v>
       </c>
-      <c r="P18" s="19">
+      <c r="P18" s="17">
         <f t="shared" si="1"/>
         <v>1250423</v>
       </c>
-      <c r="Q18" s="19">
+      <c r="Q18" s="17">
         <f t="shared" si="1"/>
         <v>1249600</v>
       </c>
-      <c r="R18" s="19">
+      <c r="R18" s="17">
         <f t="shared" si="1"/>
         <v>1247234</v>
       </c>
-      <c r="S18" s="19">
+      <c r="S18" s="17">
         <f t="shared" si="1"/>
         <v>1240463</v>
       </c>
-      <c r="T18" s="19">
+      <c r="T18" s="17">
         <f t="shared" si="1"/>
         <v>1238528</v>
       </c>
@@ -17954,35 +17954,35 @@
       <c r="L19" t="s">
         <v>457</v>
       </c>
-      <c r="M19" s="19">
+      <c r="M19" s="17">
         <f t="shared" si="3"/>
         <v>1099971</v>
       </c>
-      <c r="N19" s="19">
+      <c r="N19" s="17">
         <f t="shared" si="1"/>
         <v>1105980</v>
       </c>
-      <c r="O19" s="19">
+      <c r="O19" s="17">
         <f t="shared" si="1"/>
         <v>1109866</v>
       </c>
-      <c r="P19" s="19">
+      <c r="P19" s="17">
         <f t="shared" si="1"/>
         <v>1111872</v>
       </c>
-      <c r="Q19" s="19">
+      <c r="Q19" s="17">
         <f t="shared" si="1"/>
         <v>1112707</v>
       </c>
-      <c r="R19" s="19">
+      <c r="R19" s="17">
         <f t="shared" si="1"/>
         <v>1112773</v>
       </c>
-      <c r="S19" s="19">
+      <c r="S19" s="17">
         <f t="shared" si="1"/>
         <v>1110207</v>
       </c>
-      <c r="T19" s="19">
+      <c r="T19" s="17">
         <f t="shared" si="1"/>
         <v>1109269</v>
       </c>
@@ -18022,35 +18022,35 @@
       <c r="L20" t="s">
         <v>458</v>
       </c>
-      <c r="M20" s="19">
+      <c r="M20" s="17">
         <f t="shared" si="3"/>
         <v>1000712</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="17">
         <f t="shared" si="1"/>
         <v>1012528</v>
       </c>
-      <c r="O20" s="19">
+      <c r="O20" s="17">
         <f t="shared" si="1"/>
         <v>1022772</v>
       </c>
-      <c r="P20" s="19">
+      <c r="P20" s="17">
         <f t="shared" si="1"/>
         <v>1032261</v>
       </c>
-      <c r="Q20" s="19">
+      <c r="Q20" s="17">
         <f t="shared" si="1"/>
         <v>1042664</v>
       </c>
-      <c r="R20" s="19">
+      <c r="R20" s="17">
         <f t="shared" si="1"/>
         <v>1054532</v>
       </c>
-      <c r="S20" s="19">
+      <c r="S20" s="17">
         <f t="shared" si="1"/>
         <v>1065623</v>
       </c>
-      <c r="T20" s="19">
+      <c r="T20" s="17">
         <f t="shared" si="1"/>
         <v>1067482</v>
       </c>
@@ -18090,35 +18090,35 @@
       <c r="L21" t="s">
         <v>459</v>
       </c>
-      <c r="M21" s="19">
+      <c r="M21" s="17">
         <f t="shared" si="3"/>
         <v>1798453</v>
       </c>
-      <c r="N21" s="19">
+      <c r="N21" s="17">
         <f t="shared" si="1"/>
         <v>1804013</v>
       </c>
-      <c r="O21" s="19">
+      <c r="O21" s="17">
         <f t="shared" si="1"/>
         <v>1805868</v>
       </c>
-      <c r="P21" s="19">
+      <c r="P21" s="17">
         <f t="shared" si="1"/>
         <v>1804737</v>
       </c>
-      <c r="Q21" s="19">
+      <c r="Q21" s="17">
         <f t="shared" si="1"/>
         <v>1801332</v>
       </c>
-      <c r="R21" s="19">
+      <c r="R21" s="17">
         <f t="shared" si="1"/>
         <v>1793140</v>
       </c>
-      <c r="S21" s="19">
+      <c r="S21" s="17">
         <f t="shared" si="1"/>
         <v>1775140</v>
       </c>
-      <c r="T21" s="19">
+      <c r="T21" s="17">
         <f t="shared" si="1"/>
         <v>1770401</v>
       </c>
@@ -18158,35 +18158,35 @@
       <c r="L22" t="s">
         <v>460</v>
       </c>
-      <c r="M22" s="19">
+      <c r="M22" s="17">
         <f t="shared" si="3"/>
         <v>1277074</v>
       </c>
-      <c r="N22" s="19">
+      <c r="N22" s="17">
         <f t="shared" si="1"/>
         <v>1289106</v>
       </c>
-      <c r="O22" s="19">
+      <c r="O22" s="17">
         <f t="shared" si="1"/>
         <v>1298276</v>
       </c>
-      <c r="P22" s="19">
+      <c r="P22" s="17">
         <f t="shared" si="1"/>
         <v>1305198</v>
       </c>
-      <c r="Q22" s="19">
+      <c r="Q22" s="17">
         <f t="shared" si="1"/>
         <v>1311376</v>
       </c>
-      <c r="R22" s="19">
+      <c r="R22" s="17">
         <f t="shared" si="1"/>
         <v>1316512</v>
       </c>
-      <c r="S22" s="19">
+      <c r="S22" s="17">
         <f t="shared" si="1"/>
         <v>1317535</v>
       </c>
-      <c r="T22" s="19">
+      <c r="T22" s="17">
         <f t="shared" si="1"/>
         <v>1317124</v>
       </c>
@@ -18226,35 +18226,35 @@
       <c r="L23" t="s">
         <v>461</v>
       </c>
-      <c r="M23" s="19">
+      <c r="M23" s="17">
         <f t="shared" si="3"/>
         <v>1902200</v>
       </c>
-      <c r="N23" s="19">
+      <c r="N23" s="17">
         <f t="shared" si="1"/>
         <v>1908943</v>
       </c>
-      <c r="O23" s="19">
+      <c r="O23" s="17">
         <f t="shared" si="1"/>
         <v>1911911</v>
       </c>
-      <c r="P23" s="19">
+      <c r="P23" s="17">
         <f t="shared" si="1"/>
         <v>1912459</v>
       </c>
-      <c r="Q23" s="19">
+      <c r="Q23" s="17">
         <f t="shared" si="1"/>
         <v>1911214</v>
       </c>
-      <c r="R23" s="19">
+      <c r="R23" s="17">
         <f t="shared" si="1"/>
         <v>1906018</v>
       </c>
-      <c r="S23" s="19">
+      <c r="S23" s="17">
         <f t="shared" si="1"/>
         <v>1891768</v>
       </c>
-      <c r="T23" s="19">
+      <c r="T23" s="17">
         <f t="shared" si="1"/>
         <v>1887754</v>
       </c>
@@ -18294,35 +18294,35 @@
       <c r="L24" t="s">
         <v>462</v>
       </c>
-      <c r="M24" s="19">
+      <c r="M24" s="17">
         <f t="shared" si="3"/>
         <v>3992651</v>
       </c>
-      <c r="N24" s="19">
+      <c r="N24" s="17">
         <f t="shared" si="1"/>
         <v>3945867</v>
       </c>
-      <c r="O24" s="19">
+      <c r="O24" s="17">
         <f t="shared" si="1"/>
         <v>3900071</v>
       </c>
-      <c r="P24" s="19">
+      <c r="P24" s="17">
         <f t="shared" si="1"/>
         <v>3858851</v>
       </c>
-      <c r="Q24" s="19">
+      <c r="Q24" s="17">
         <f t="shared" si="1"/>
         <v>3816517</v>
       </c>
-      <c r="R24" s="19">
+      <c r="R24" s="17">
         <f t="shared" si="1"/>
         <v>3757721</v>
       </c>
-      <c r="S24" s="19">
+      <c r="S24" s="17">
         <f t="shared" si="1"/>
         <v>3665714</v>
       </c>
-      <c r="T24" s="19">
+      <c r="T24" s="17">
         <f t="shared" si="1"/>
         <v>3644826</v>
       </c>
@@ -18362,35 +18362,35 @@
       <c r="L25" t="s">
         <v>463</v>
       </c>
-      <c r="M25" s="19">
+      <c r="M25" s="17">
         <f t="shared" si="3"/>
         <v>2320865</v>
       </c>
-      <c r="N25" s="19">
+      <c r="N25" s="17">
         <f t="shared" si="1"/>
         <v>2354515</v>
       </c>
-      <c r="O25" s="19">
+      <c r="O25" s="17">
         <f t="shared" si="1"/>
         <v>2383338</v>
       </c>
-      <c r="P25" s="19">
+      <c r="P25" s="17">
         <f t="shared" si="1"/>
         <v>2412055</v>
       </c>
-      <c r="Q25" s="19">
+      <c r="Q25" s="17">
         <f t="shared" si="1"/>
         <v>2445513</v>
       </c>
-      <c r="R25" s="19">
+      <c r="R25" s="17">
         <f t="shared" si="1"/>
         <v>2480872</v>
       </c>
-      <c r="S25" s="19">
+      <c r="S25" s="17">
         <f t="shared" si="1"/>
         <v>2508276</v>
       </c>
-      <c r="T25" s="19">
+      <c r="T25" s="17">
         <f t="shared" si="1"/>
         <v>2511917</v>
       </c>
@@ -18430,35 +18430,35 @@
       <c r="L26" t="s">
         <v>464</v>
       </c>
-      <c r="M26" s="19">
+      <c r="M26" s="17">
         <f t="shared" si="3"/>
         <v>721341</v>
       </c>
-      <c r="N26" s="19">
+      <c r="N26" s="17">
         <f t="shared" si="1"/>
         <v>717191</v>
       </c>
-      <c r="O26" s="19">
+      <c r="O26" s="17">
         <f t="shared" si="1"/>
         <v>712520</v>
       </c>
-      <c r="P26" s="19">
+      <c r="P26" s="17">
         <f t="shared" si="1"/>
         <v>707849</v>
       </c>
-      <c r="Q26" s="19">
+      <c r="Q26" s="17">
         <f t="shared" si="1"/>
         <v>703006</v>
       </c>
-      <c r="R26" s="19">
+      <c r="R26" s="17">
         <f t="shared" si="1"/>
         <v>696447</v>
       </c>
-      <c r="S26" s="19">
+      <c r="S26" s="17">
         <f t="shared" si="1"/>
         <v>685650</v>
       </c>
-      <c r="T26" s="19">
+      <c r="T26" s="17">
         <f t="shared" si="1"/>
         <v>682986</v>
       </c>
@@ -18498,35 +18498,35 @@
       <c r="L27" t="s">
         <v>465</v>
       </c>
-      <c r="M27" s="19">
+      <c r="M27" s="17">
         <f t="shared" si="3"/>
         <v>1994063</v>
       </c>
-      <c r="N27" s="19">
+      <c r="N27" s="17">
         <f t="shared" si="1"/>
         <v>1976290</v>
       </c>
-      <c r="O27" s="19">
+      <c r="O27" s="17">
         <f t="shared" si="1"/>
         <v>1957818</v>
       </c>
-      <c r="P27" s="19">
+      <c r="P27" s="17">
         <f t="shared" si="1"/>
         <v>1939747</v>
       </c>
-      <c r="Q27" s="19">
+      <c r="Q27" s="17">
         <f t="shared" si="1"/>
         <v>1919608</v>
       </c>
-      <c r="R27" s="19">
+      <c r="R27" s="17">
         <f t="shared" si="1"/>
         <v>1891643</v>
       </c>
-      <c r="S27" s="19">
+      <c r="S27" s="17">
         <f t="shared" si="1"/>
         <v>1850072</v>
       </c>
-      <c r="T27" s="19">
+      <c r="T27" s="17">
         <f t="shared" si="1"/>
         <v>1841179</v>
       </c>
@@ -18566,35 +18566,35 @@
       <c r="L28" t="s">
         <v>466</v>
       </c>
-      <c r="M28" s="19">
+      <c r="M28" s="17">
         <f t="shared" si="3"/>
         <v>4061065</v>
       </c>
-      <c r="N28" s="19">
+      <c r="N28" s="17">
         <f t="shared" si="1"/>
         <v>4068110</v>
       </c>
-      <c r="O28" s="19">
+      <c r="O28" s="17">
         <f t="shared" si="1"/>
         <v>4069471</v>
       </c>
-      <c r="P28" s="19">
+      <c r="P28" s="17">
         <f t="shared" si="1"/>
         <v>4067560</v>
       </c>
-      <c r="Q28" s="19">
+      <c r="Q28" s="17">
         <f t="shared" si="1"/>
         <v>4062274</v>
       </c>
-      <c r="R28" s="19">
+      <c r="R28" s="17">
         <f t="shared" si="1"/>
         <v>4047884</v>
       </c>
-      <c r="S28" s="19">
+      <c r="S28" s="17">
         <f t="shared" si="1"/>
         <v>4007749</v>
       </c>
-      <c r="T28" s="19">
+      <c r="T28" s="17">
         <f t="shared" si="1"/>
         <v>3998724</v>
       </c>
@@ -18634,35 +18634,35 @@
       <c r="L29" t="s">
         <v>467</v>
       </c>
-      <c r="M29" s="19">
+      <c r="M29" s="17">
         <f t="shared" si="3"/>
         <v>1167033</v>
       </c>
-      <c r="N29" s="19">
+      <c r="N29" s="17">
         <f t="shared" ref="N29:N50" si="4">SUMIF($J$13:$J$413,$L29,C$13:C$413)</f>
         <v>1162396</v>
       </c>
-      <c r="O29" s="19">
+      <c r="O29" s="17">
         <f t="shared" ref="O29:O50" si="5">SUMIF($J$13:$J$413,$L29,D$13:D$413)</f>
         <v>1153235</v>
       </c>
-      <c r="P29" s="19">
+      <c r="P29" s="17">
         <f t="shared" ref="P29:P50" si="6">SUMIF($J$13:$J$413,$L29,E$13:E$413)</f>
         <v>1139369</v>
       </c>
-      <c r="Q29" s="19">
+      <c r="Q29" s="17">
         <f t="shared" ref="Q29:Q50" si="7">SUMIF($J$13:$J$413,$L29,F$13:F$413)</f>
         <v>1120162</v>
       </c>
-      <c r="R29" s="19">
+      <c r="R29" s="17">
         <f t="shared" ref="R29:R50" si="8">SUMIF($J$13:$J$413,$L29,G$13:G$413)</f>
         <v>1093670</v>
       </c>
-      <c r="S29" s="19">
+      <c r="S29" s="17">
         <f t="shared" ref="S29:S50" si="9">SUMIF($J$13:$J$413,$L29,H$13:H$413)</f>
         <v>1056347</v>
       </c>
-      <c r="T29" s="19">
+      <c r="T29" s="17">
         <f t="shared" ref="T29:T50" si="10">SUMIF($J$13:$J$413,$L29,I$13:I$413)</f>
         <v>1047262</v>
       </c>
@@ -18702,35 +18702,35 @@
       <c r="L30" t="s">
         <v>468</v>
       </c>
-      <c r="M30" s="19">
+      <c r="M30" s="17">
         <f t="shared" si="3"/>
         <v>1146788</v>
       </c>
-      <c r="N30" s="19">
+      <c r="N30" s="17">
         <f t="shared" si="4"/>
         <v>1158742</v>
       </c>
-      <c r="O30" s="19">
+      <c r="O30" s="17">
         <f t="shared" si="5"/>
         <v>1169518</v>
       </c>
-      <c r="P30" s="19">
+      <c r="P30" s="17">
         <f t="shared" si="6"/>
         <v>1180124</v>
       </c>
-      <c r="Q30" s="19">
+      <c r="Q30" s="17">
         <f t="shared" si="7"/>
         <v>1192226</v>
       </c>
-      <c r="R30" s="19">
+      <c r="R30" s="17">
         <f t="shared" si="8"/>
         <v>1205435</v>
       </c>
-      <c r="S30" s="19">
+      <c r="S30" s="17">
         <f t="shared" si="9"/>
         <v>1217605</v>
       </c>
-      <c r="T30" s="19">
+      <c r="T30" s="17">
         <f t="shared" si="10"/>
         <v>1219823</v>
       </c>
@@ -18770,35 +18770,35 @@
       <c r="L31" t="s">
         <v>469</v>
       </c>
-      <c r="M31" s="19">
+      <c r="M31" s="17">
         <f t="shared" si="3"/>
         <v>1484617</v>
       </c>
-      <c r="N31" s="19">
+      <c r="N31" s="17">
         <f t="shared" si="4"/>
         <v>1507073</v>
       </c>
-      <c r="O31" s="19">
+      <c r="O31" s="17">
         <f t="shared" si="5"/>
         <v>1527341</v>
       </c>
-      <c r="P31" s="19">
+      <c r="P31" s="17">
         <f t="shared" si="6"/>
         <v>1547018</v>
       </c>
-      <c r="Q31" s="19">
+      <c r="Q31" s="17">
         <f t="shared" si="7"/>
         <v>1568937</v>
       </c>
-      <c r="R31" s="19">
+      <c r="R31" s="17">
         <f t="shared" si="8"/>
         <v>1591224</v>
       </c>
-      <c r="S31" s="19">
+      <c r="S31" s="17">
         <f t="shared" si="9"/>
         <v>1607890</v>
       </c>
-      <c r="T31" s="19">
+      <c r="T31" s="17">
         <f t="shared" si="10"/>
         <v>1609675</v>
       </c>
@@ -18838,35 +18838,35 @@
       <c r="L32" t="s">
         <v>470</v>
       </c>
-      <c r="M32" s="19">
+      <c r="M32" s="17">
         <f t="shared" si="3"/>
         <v>1665137</v>
       </c>
-      <c r="N32" s="19">
+      <c r="N32" s="17">
         <f t="shared" si="4"/>
         <v>1666181</v>
       </c>
-      <c r="O32" s="19">
+      <c r="O32" s="17">
         <f t="shared" si="5"/>
         <v>1662579</v>
       </c>
-      <c r="P32" s="19">
+      <c r="P32" s="17">
         <f t="shared" si="6"/>
         <v>1655488</v>
       </c>
-      <c r="Q32" s="19">
+      <c r="Q32" s="17">
         <f t="shared" si="7"/>
         <v>1645908</v>
       </c>
-      <c r="R32" s="19">
+      <c r="R32" s="17">
         <f t="shared" si="8"/>
         <v>1630802</v>
       </c>
-      <c r="S32" s="19">
+      <c r="S32" s="17">
         <f t="shared" si="9"/>
         <v>1603711</v>
       </c>
-      <c r="T32" s="19">
+      <c r="T32" s="17">
         <f t="shared" si="10"/>
         <v>1596396</v>
       </c>
@@ -18906,35 +18906,35 @@
       <c r="L33" t="s">
         <v>471</v>
       </c>
-      <c r="M33" s="19">
+      <c r="M33" s="17">
         <f t="shared" si="3"/>
         <v>2047856</v>
       </c>
-      <c r="N33" s="19">
+      <c r="N33" s="17">
         <f t="shared" si="4"/>
         <v>2062048</v>
       </c>
-      <c r="O33" s="19">
+      <c r="O33" s="17">
         <f t="shared" si="5"/>
         <v>2074878</v>
       </c>
-      <c r="P33" s="19">
+      <c r="P33" s="17">
         <f t="shared" si="6"/>
         <v>2089080</v>
       </c>
-      <c r="Q33" s="19">
+      <c r="Q33" s="17">
         <f t="shared" si="7"/>
         <v>2107207</v>
       </c>
-      <c r="R33" s="19">
+      <c r="R33" s="17">
         <f t="shared" si="8"/>
         <v>2127925</v>
       </c>
-      <c r="S33" s="19">
+      <c r="S33" s="17">
         <f t="shared" si="9"/>
         <v>2146365</v>
       </c>
-      <c r="T33" s="19">
+      <c r="T33" s="17">
         <f t="shared" si="10"/>
         <v>2149805</v>
       </c>
@@ -18974,35 +18974,35 @@
       <c r="L34" t="s">
         <v>472</v>
       </c>
-      <c r="M34" s="19">
+      <c r="M34" s="17">
         <f t="shared" si="3"/>
         <v>1609484</v>
       </c>
-      <c r="N34" s="19">
+      <c r="N34" s="17">
         <f t="shared" si="4"/>
         <v>1626906</v>
       </c>
-      <c r="O34" s="19">
+      <c r="O34" s="17">
         <f t="shared" si="5"/>
         <v>1642751</v>
       </c>
-      <c r="P34" s="19">
+      <c r="P34" s="17">
         <f t="shared" si="6"/>
         <v>1658457</v>
       </c>
-      <c r="Q34" s="19">
+      <c r="Q34" s="17">
         <f t="shared" si="7"/>
         <v>1675887</v>
       </c>
-      <c r="R34" s="19">
+      <c r="R34" s="17">
         <f t="shared" si="8"/>
         <v>1694324</v>
       </c>
-      <c r="S34" s="19">
+      <c r="S34" s="17">
         <f t="shared" si="9"/>
         <v>1708702</v>
       </c>
-      <c r="T34" s="19">
+      <c r="T34" s="17">
         <f t="shared" si="10"/>
         <v>1710914</v>
       </c>
@@ -19042,35 +19042,35 @@
       <c r="L35" t="s">
         <v>473</v>
       </c>
-      <c r="M35" s="19">
+      <c r="M35" s="17">
         <f t="shared" si="3"/>
         <v>2523531</v>
       </c>
-      <c r="N35" s="19">
+      <c r="N35" s="17">
         <f t="shared" si="4"/>
         <v>2532591</v>
       </c>
-      <c r="O35" s="19">
+      <c r="O35" s="17">
         <f t="shared" si="5"/>
         <v>2537372</v>
       </c>
-      <c r="P35" s="19">
+      <c r="P35" s="17">
         <f t="shared" si="6"/>
         <v>2538766</v>
       </c>
-      <c r="Q35" s="19">
+      <c r="Q35" s="17">
         <f t="shared" si="7"/>
         <v>2539400</v>
       </c>
-      <c r="R35" s="19">
+      <c r="R35" s="17">
         <f t="shared" si="8"/>
         <v>2538559</v>
       </c>
-      <c r="S35" s="19">
+      <c r="S35" s="17">
         <f t="shared" si="9"/>
         <v>2528526</v>
       </c>
-      <c r="T35" s="19">
+      <c r="T35" s="17">
         <f t="shared" si="10"/>
         <v>2525333</v>
       </c>
@@ -19110,35 +19110,35 @@
       <c r="L36" t="s">
         <v>474</v>
       </c>
-      <c r="M36" s="19">
+      <c r="M36" s="17">
         <f t="shared" si="3"/>
         <v>5121670</v>
       </c>
-      <c r="N36" s="19">
+      <c r="N36" s="17">
         <f t="shared" si="4"/>
         <v>5143542</v>
       </c>
-      <c r="O36" s="19">
+      <c r="O36" s="17">
         <f t="shared" si="5"/>
         <v>5158849</v>
       </c>
-      <c r="P36" s="19">
+      <c r="P36" s="17">
         <f t="shared" si="6"/>
         <v>5171896</v>
       </c>
-      <c r="Q36" s="19">
+      <c r="Q36" s="17">
         <f t="shared" si="7"/>
         <v>5188480</v>
       </c>
-      <c r="R36" s="19">
+      <c r="R36" s="17">
         <f t="shared" si="8"/>
         <v>5203755</v>
       </c>
-      <c r="S36" s="19">
+      <c r="S36" s="17">
         <f t="shared" si="9"/>
         <v>5203764</v>
       </c>
-      <c r="T36" s="19">
+      <c r="T36" s="17">
         <f t="shared" si="10"/>
         <v>5202321</v>
       </c>
@@ -19178,35 +19178,35 @@
       <c r="L37" t="s">
         <v>475</v>
       </c>
-      <c r="M37" s="19">
+      <c r="M37" s="17">
         <f t="shared" si="3"/>
         <v>4438751</v>
       </c>
-      <c r="N37" s="19">
+      <c r="N37" s="17">
         <f t="shared" si="4"/>
         <v>4457231</v>
       </c>
-      <c r="O37" s="19">
+      <c r="O37" s="17">
         <f t="shared" si="5"/>
         <v>4469098</v>
       </c>
-      <c r="P37" s="19">
+      <c r="P37" s="17">
         <f t="shared" si="6"/>
         <v>4477562</v>
       </c>
-      <c r="Q37" s="19">
+      <c r="Q37" s="17">
         <f t="shared" si="7"/>
         <v>4484833</v>
       </c>
-      <c r="R37" s="19">
+      <c r="R37" s="17">
         <f t="shared" si="8"/>
         <v>4487050</v>
       </c>
-      <c r="S37" s="19">
+      <c r="S37" s="17">
         <f t="shared" si="9"/>
         <v>4473404</v>
       </c>
-      <c r="T37" s="19">
+      <c r="T37" s="17">
         <f t="shared" si="10"/>
         <v>4468904</v>
       </c>
@@ -19246,35 +19246,35 @@
       <c r="L38" t="s">
         <v>476</v>
       </c>
-      <c r="M38" s="19">
+      <c r="M38" s="17">
         <f t="shared" si="3"/>
         <v>2643150</v>
       </c>
-      <c r="N38" s="19">
+      <c r="N38" s="17">
         <f t="shared" si="4"/>
         <v>2650628</v>
       </c>
-      <c r="O38" s="19">
+      <c r="O38" s="17">
         <f t="shared" si="5"/>
         <v>2652851</v>
       </c>
-      <c r="P38" s="19">
+      <c r="P38" s="17">
         <f t="shared" si="6"/>
         <v>2650275</v>
       </c>
-      <c r="Q38" s="19">
+      <c r="Q38" s="17">
         <f t="shared" si="7"/>
         <v>2645705</v>
       </c>
-      <c r="R38" s="19">
+      <c r="R38" s="17">
         <f t="shared" si="8"/>
         <v>2640110</v>
       </c>
-      <c r="S38" s="19">
+      <c r="S38" s="17">
         <f t="shared" si="9"/>
         <v>2627458</v>
       </c>
-      <c r="T38" s="19">
+      <c r="T38" s="17">
         <f t="shared" si="10"/>
         <v>2623619</v>
       </c>
@@ -19314,35 +19314,35 @@
       <c r="L39" t="s">
         <v>477</v>
       </c>
-      <c r="M39" s="19">
+      <c r="M39" s="17">
         <f t="shared" si="3"/>
         <v>2096052</v>
       </c>
-      <c r="N39" s="19">
+      <c r="N39" s="17">
         <f t="shared" si="4"/>
         <v>2097554</v>
       </c>
-      <c r="O39" s="19">
+      <c r="O39" s="17">
         <f t="shared" si="5"/>
         <v>2094433</v>
       </c>
-      <c r="P39" s="19">
+      <c r="P39" s="17">
         <f t="shared" si="6"/>
         <v>2088413</v>
       </c>
-      <c r="Q39" s="19">
+      <c r="Q39" s="17">
         <f t="shared" si="7"/>
         <v>2082158</v>
       </c>
-      <c r="R39" s="19">
+      <c r="R39" s="17">
         <f t="shared" si="8"/>
         <v>2074519</v>
       </c>
-      <c r="S39" s="19">
+      <c r="S39" s="17">
         <f t="shared" si="9"/>
         <v>2059525</v>
       </c>
-      <c r="T39" s="19">
+      <c r="T39" s="17">
         <f t="shared" si="10"/>
         <v>2055310</v>
       </c>
@@ -19382,35 +19382,35 @@
       <c r="L40" t="s">
         <v>478</v>
       </c>
-      <c r="M40" s="19">
+      <c r="M40" s="17">
         <f t="shared" si="3"/>
         <v>3603247</v>
       </c>
-      <c r="N40" s="19">
+      <c r="N40" s="17">
         <f t="shared" si="4"/>
         <v>3610305</v>
       </c>
-      <c r="O40" s="19">
+      <c r="O40" s="17">
         <f t="shared" si="5"/>
         <v>3611339</v>
       </c>
-      <c r="P40" s="19">
+      <c r="P40" s="17">
         <f t="shared" si="6"/>
         <v>3608451</v>
       </c>
-      <c r="Q40" s="19">
+      <c r="Q40" s="17">
         <f t="shared" si="7"/>
         <v>3606022</v>
       </c>
-      <c r="R40" s="19">
+      <c r="R40" s="17">
         <f t="shared" si="8"/>
         <v>3602014</v>
       </c>
-      <c r="S40" s="19">
+      <c r="S40" s="17">
         <f t="shared" si="9"/>
         <v>3587260</v>
       </c>
-      <c r="T40" s="19">
+      <c r="T40" s="17">
         <f t="shared" si="10"/>
         <v>3582497</v>
       </c>
@@ -19450,35 +19450,35 @@
       <c r="L41" t="s">
         <v>479</v>
       </c>
-      <c r="M41" s="19">
+      <c r="M41" s="17">
         <f t="shared" si="3"/>
         <v>1395050</v>
       </c>
-      <c r="N41" s="19">
+      <c r="N41" s="17">
         <f t="shared" si="4"/>
         <v>1412325</v>
       </c>
-      <c r="O41" s="19">
+      <c r="O41" s="17">
         <f t="shared" si="5"/>
         <v>1427796</v>
       </c>
-      <c r="P41" s="19">
+      <c r="P41" s="17">
         <f t="shared" si="6"/>
         <v>1442436</v>
       </c>
-      <c r="Q41" s="19">
+      <c r="Q41" s="17">
         <f t="shared" si="7"/>
         <v>1458316</v>
       </c>
-      <c r="R41" s="19">
+      <c r="R41" s="17">
         <f t="shared" si="8"/>
         <v>1475851</v>
       </c>
-      <c r="S41" s="19">
+      <c r="S41" s="17">
         <f t="shared" si="9"/>
         <v>1492711</v>
       </c>
-      <c r="T41" s="19">
+      <c r="T41" s="17">
         <f t="shared" si="10"/>
         <v>1495885</v>
       </c>
@@ -19518,35 +19518,35 @@
       <c r="L42" t="s">
         <v>480</v>
       </c>
-      <c r="M42" s="19">
+      <c r="M42" s="17">
         <f t="shared" si="3"/>
         <v>593599</v>
       </c>
-      <c r="N42" s="19">
+      <c r="N42" s="17">
         <f t="shared" si="4"/>
         <v>593099</v>
       </c>
-      <c r="O42" s="19">
+      <c r="O42" s="17">
         <f t="shared" si="5"/>
         <v>589933</v>
       </c>
-      <c r="P42" s="19">
+      <c r="P42" s="17">
         <f t="shared" si="6"/>
         <v>583607</v>
       </c>
-      <c r="Q42" s="19">
+      <c r="Q42" s="17">
         <f t="shared" si="7"/>
         <v>573882</v>
       </c>
-      <c r="R42" s="19">
+      <c r="R42" s="17">
         <f t="shared" si="8"/>
         <v>559585</v>
       </c>
-      <c r="S42" s="19">
+      <c r="S42" s="17">
         <f t="shared" si="9"/>
         <v>536843</v>
       </c>
-      <c r="T42" s="19">
+      <c r="T42" s="17">
         <f t="shared" si="10"/>
         <v>531007</v>
       </c>
@@ -19586,35 +19586,35 @@
       <c r="L43" t="s">
         <v>481</v>
       </c>
-      <c r="M43" s="19">
+      <c r="M43" s="17">
         <f t="shared" si="3"/>
         <v>1969788</v>
       </c>
-      <c r="N43" s="19">
+      <c r="N43" s="17">
         <f t="shared" si="4"/>
         <v>1990969</v>
       </c>
-      <c r="O43" s="19">
+      <c r="O43" s="17">
         <f t="shared" si="5"/>
         <v>2008963</v>
       </c>
-      <c r="P43" s="19">
+      <c r="P43" s="17">
         <f t="shared" si="6"/>
         <v>2024266</v>
       </c>
-      <c r="Q43" s="19">
+      <c r="Q43" s="17">
         <f t="shared" si="7"/>
         <v>2038460</v>
       </c>
-      <c r="R43" s="19">
+      <c r="R43" s="17">
         <f t="shared" si="8"/>
         <v>2050841</v>
       </c>
-      <c r="S43" s="19">
+      <c r="S43" s="17">
         <f t="shared" si="9"/>
         <v>2057421</v>
       </c>
-      <c r="T43" s="19">
+      <c r="T43" s="17">
         <f t="shared" si="10"/>
         <v>2057952</v>
       </c>
@@ -19654,35 +19654,35 @@
       <c r="L44" t="s">
         <v>482</v>
       </c>
-      <c r="M44" s="19">
+      <c r="M44" s="17">
         <f t="shared" si="3"/>
         <v>953851</v>
       </c>
-      <c r="N44" s="19">
+      <c r="N44" s="17">
         <f t="shared" si="4"/>
         <v>961738</v>
       </c>
-      <c r="O44" s="19">
+      <c r="O44" s="17">
         <f t="shared" si="5"/>
         <v>968188</v>
       </c>
-      <c r="P44" s="19">
+      <c r="P44" s="17">
         <f t="shared" si="6"/>
         <v>973593</v>
       </c>
-      <c r="Q44" s="19">
+      <c r="Q44" s="17">
         <f t="shared" si="7"/>
         <v>979356</v>
       </c>
-      <c r="R44" s="19">
+      <c r="R44" s="17">
         <f t="shared" si="8"/>
         <v>985667</v>
       </c>
-      <c r="S44" s="19">
+      <c r="S44" s="17">
         <f t="shared" si="9"/>
         <v>989983</v>
       </c>
-      <c r="T44" s="19">
+      <c r="T44" s="17">
         <f t="shared" si="10"/>
         <v>990509</v>
       </c>
@@ -19722,35 +19722,35 @@
       <c r="L45" t="s">
         <v>483</v>
       </c>
-      <c r="M45" s="19">
+      <c r="M45" s="17">
         <f t="shared" si="3"/>
         <v>1584997</v>
       </c>
-      <c r="N45" s="19">
+      <c r="N45" s="17">
         <f t="shared" si="4"/>
         <v>1585162</v>
       </c>
-      <c r="O45" s="19">
+      <c r="O45" s="17">
         <f t="shared" si="5"/>
         <v>1585393</v>
       </c>
-      <c r="P45" s="19">
+      <c r="P45" s="17">
         <f t="shared" si="6"/>
         <v>1588902</v>
       </c>
-      <c r="Q45" s="19">
+      <c r="Q45" s="17">
         <f t="shared" si="7"/>
         <v>1596481</v>
       </c>
-      <c r="R45" s="19">
+      <c r="R45" s="17">
         <f t="shared" si="8"/>
         <v>1602849</v>
       </c>
-      <c r="S45" s="19">
+      <c r="S45" s="17">
         <f t="shared" si="9"/>
         <v>1600347</v>
       </c>
-      <c r="T45" s="19">
+      <c r="T45" s="17">
         <f t="shared" si="10"/>
         <v>1598199</v>
       </c>
@@ -19790,35 +19790,35 @@
       <c r="L46" t="s">
         <v>484</v>
       </c>
-      <c r="M46" s="19">
+      <c r="M46" s="17">
         <f t="shared" si="3"/>
         <v>1224694</v>
       </c>
-      <c r="N46" s="19">
+      <c r="N46" s="17">
         <f t="shared" si="4"/>
         <v>1248142</v>
       </c>
-      <c r="O46" s="19">
+      <c r="O46" s="17">
         <f t="shared" si="5"/>
         <v>1274782</v>
       </c>
-      <c r="P46" s="19">
+      <c r="P46" s="17">
         <f t="shared" si="6"/>
         <v>1305861</v>
       </c>
-      <c r="Q46" s="19">
+      <c r="Q46" s="17">
         <f t="shared" si="7"/>
         <v>1342988</v>
       </c>
-      <c r="R46" s="19">
+      <c r="R46" s="17">
         <f t="shared" si="8"/>
         <v>1385097</v>
       </c>
-      <c r="S46" s="19">
+      <c r="S46" s="17">
         <f t="shared" si="9"/>
         <v>1428336</v>
       </c>
-      <c r="T46" s="19">
+      <c r="T46" s="17">
         <f t="shared" si="10"/>
         <v>1436445</v>
       </c>
@@ -19858,35 +19858,35 @@
       <c r="L47" t="s">
         <v>485</v>
       </c>
-      <c r="M47" s="19">
+      <c r="M47" s="17">
         <f t="shared" si="3"/>
         <v>976684</v>
       </c>
-      <c r="N47" s="19">
+      <c r="N47" s="17">
         <f t="shared" si="4"/>
         <v>985215</v>
       </c>
-      <c r="O47" s="19">
+      <c r="O47" s="17">
         <f t="shared" si="5"/>
         <v>994746</v>
       </c>
-      <c r="P47" s="19">
+      <c r="P47" s="17">
         <f t="shared" si="6"/>
         <v>1006658</v>
       </c>
-      <c r="Q47" s="19">
+      <c r="Q47" s="17">
         <f t="shared" si="7"/>
         <v>1020651</v>
       </c>
-      <c r="R47" s="19">
+      <c r="R47" s="17">
         <f t="shared" si="8"/>
         <v>1033553</v>
       </c>
-      <c r="S47" s="19">
+      <c r="S47" s="17">
         <f t="shared" si="9"/>
         <v>1042270</v>
       </c>
-      <c r="T47" s="19">
+      <c r="T47" s="17">
         <f t="shared" si="10"/>
         <v>1043293</v>
       </c>
@@ -19926,35 +19926,35 @@
       <c r="L48" t="s">
         <v>486</v>
       </c>
-      <c r="M48" s="19">
+      <c r="M48" s="17">
         <f t="shared" si="3"/>
         <v>2012673</v>
       </c>
-      <c r="N48" s="19">
+      <c r="N48" s="17">
         <f t="shared" si="4"/>
         <v>2039109</v>
       </c>
-      <c r="O48" s="19">
+      <c r="O48" s="17">
         <f t="shared" si="5"/>
         <v>2065747</v>
       </c>
-      <c r="P48" s="19">
+      <c r="P48" s="17">
         <f t="shared" si="6"/>
         <v>2095021</v>
       </c>
-      <c r="Q48" s="19">
+      <c r="Q48" s="17">
         <f t="shared" si="7"/>
         <v>2130055</v>
       </c>
-      <c r="R48" s="19">
+      <c r="R48" s="17">
         <f t="shared" si="8"/>
         <v>2168539</v>
       </c>
-      <c r="S48" s="19">
+      <c r="S48" s="17">
         <f t="shared" si="9"/>
         <v>2202815</v>
       </c>
-      <c r="T48" s="19">
+      <c r="T48" s="17">
         <f t="shared" si="10"/>
         <v>2208321</v>
       </c>
@@ -19994,35 +19994,35 @@
       <c r="L49" t="s">
         <v>487</v>
       </c>
-      <c r="M49" s="19">
+      <c r="M49" s="17">
         <f t="shared" si="3"/>
         <v>2737522</v>
       </c>
-      <c r="N49" s="19">
+      <c r="N49" s="17">
         <f t="shared" si="4"/>
         <v>2767148</v>
       </c>
-      <c r="O49" s="19">
+      <c r="O49" s="17">
         <f t="shared" si="5"/>
         <v>2793255</v>
       </c>
-      <c r="P49" s="19">
+      <c r="P49" s="17">
         <f t="shared" si="6"/>
         <v>2820035</v>
       </c>
-      <c r="Q49" s="19">
+      <c r="Q49" s="17">
         <f t="shared" si="7"/>
         <v>2849766</v>
       </c>
-      <c r="R49" s="19">
+      <c r="R49" s="17">
         <f t="shared" si="8"/>
         <v>2878070</v>
       </c>
-      <c r="S49" s="19">
+      <c r="S49" s="17">
         <f t="shared" si="9"/>
         <v>2895322</v>
       </c>
-      <c r="T49" s="19">
+      <c r="T49" s="17">
         <f t="shared" si="10"/>
         <v>2896712</v>
       </c>
@@ -20062,35 +20062,35 @@
       <c r="L50" t="s">
         <v>488</v>
       </c>
-      <c r="M50" s="19">
+      <c r="M50" s="17">
         <f t="shared" si="3"/>
         <v>1987740</v>
       </c>
-      <c r="N50" s="19">
+      <c r="N50" s="17">
         <f t="shared" si="4"/>
         <v>2012889</v>
       </c>
-      <c r="O50" s="19">
+      <c r="O50" s="17">
         <f t="shared" si="5"/>
         <v>2037244</v>
       </c>
-      <c r="P50" s="19">
+      <c r="P50" s="17">
         <f t="shared" si="6"/>
         <v>2063119</v>
       </c>
-      <c r="Q50" s="19">
+      <c r="Q50" s="17">
         <f t="shared" si="7"/>
         <v>2092065</v>
       </c>
-      <c r="R50" s="19">
+      <c r="R50" s="17">
         <f t="shared" si="8"/>
         <v>2120688</v>
       </c>
-      <c r="S50" s="19">
+      <c r="S50" s="17">
         <f t="shared" si="9"/>
         <v>2141165</v>
       </c>
-      <c r="T50" s="19">
+      <c r="T50" s="17">
         <f t="shared" si="10"/>
         <v>2143145</v>
       </c>
@@ -32072,6 +32072,40 @@
       <c r="J413" t="str">
         <f t="shared" si="16"/>
         <v>DEG0</v>
+      </c>
+    </row>
+    <row r="414" spans="1:10" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B414" s="17">
+        <f t="shared" ref="B414:H414" si="17">SUM(B13:B413)</f>
+        <v>82669724</v>
+      </c>
+      <c r="C414" s="17">
+        <f t="shared" si="17"/>
+        <v>82983422</v>
+      </c>
+      <c r="D414" s="17">
+        <f t="shared" si="17"/>
+        <v>83178426</v>
+      </c>
+      <c r="E414" s="17">
+        <f t="shared" si="17"/>
+        <v>83318670</v>
+      </c>
+      <c r="F414" s="17">
+        <f t="shared" si="17"/>
+        <v>83453697</v>
+      </c>
+      <c r="G414" s="17">
+        <f t="shared" si="17"/>
+        <v>83482307</v>
+      </c>
+      <c r="H414" s="17">
+        <f t="shared" si="17"/>
+        <v>83135181</v>
+      </c>
+      <c r="I414" s="17">
+        <f>SUM(I13:I413)</f>
+        <v>83019213</v>
       </c>
     </row>
     <row r="415" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>